<commit_message>
add simulation with jk flip flops and k maps
</commit_message>
<xml_diff>
--- a/lab2/ads-prep.xlsx
+++ b/lab2/ads-prep.xlsx
@@ -7,16 +7,15 @@
     <workbookView xWindow="240" yWindow="45" windowWidth="21075" windowHeight="10035"/>
   </bookViews>
   <sheets>
-    <sheet name="Truth Table" sheetId="1" r:id="rId1"/>
-    <sheet name="K-Maps" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="D K-Maps" sheetId="1" r:id="rId1"/>
+    <sheet name="JK K-Maps" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="12">
   <si>
     <t>Q0</t>
   </si>
@@ -34,6 +33,24 @@
   </si>
   <si>
     <t>x</t>
+  </si>
+  <si>
+    <t>K0</t>
+  </si>
+  <si>
+    <t>K1</t>
+  </si>
+  <si>
+    <t>J2</t>
+  </si>
+  <si>
+    <t>J1</t>
+  </si>
+  <si>
+    <t>J0</t>
+  </si>
+  <si>
+    <t>K2</t>
   </si>
 </sst>
 </file>
@@ -61,12 +78,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="13">
@@ -215,7 +238,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -225,9 +248,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -271,6 +291,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -575,7 +599,7 @@
   <dimension ref="A1:R167"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="N26" sqref="N26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -614,1060 +638,1060 @@
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A2" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="19">
-        <v>0</v>
-      </c>
-      <c r="E2" s="20">
-        <v>0</v>
-      </c>
-      <c r="F2" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="J2" s="13" t="s">
+      <c r="A2" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="16">
+        <v>0</v>
+      </c>
+      <c r="E2" s="17">
+        <v>0</v>
+      </c>
+      <c r="F2" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="J2" s="10" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="19">
-        <v>0</v>
-      </c>
-      <c r="B3" s="19">
-        <v>0</v>
-      </c>
-      <c r="C3" s="19">
-        <v>0</v>
-      </c>
-      <c r="D3" s="19">
-        <v>0</v>
-      </c>
-      <c r="E3" s="20">
-        <v>1</v>
-      </c>
-      <c r="F3" s="19">
-        <v>0</v>
-      </c>
-      <c r="G3" s="19">
-        <v>0</v>
-      </c>
-      <c r="H3" s="19">
-        <v>1</v>
-      </c>
-      <c r="J3" s="16"/>
-      <c r="K3" s="14">
-        <v>0</v>
-      </c>
-      <c r="L3" s="14">
-        <v>1</v>
-      </c>
-      <c r="M3" s="14">
+      <c r="A3" s="16">
+        <v>0</v>
+      </c>
+      <c r="B3" s="16">
+        <v>0</v>
+      </c>
+      <c r="C3" s="16">
+        <v>0</v>
+      </c>
+      <c r="D3" s="16">
+        <v>0</v>
+      </c>
+      <c r="E3" s="17">
+        <v>1</v>
+      </c>
+      <c r="F3" s="16">
+        <v>0</v>
+      </c>
+      <c r="G3" s="16">
+        <v>0</v>
+      </c>
+      <c r="H3" s="16">
+        <v>1</v>
+      </c>
+      <c r="J3" s="13"/>
+      <c r="K3" s="11">
+        <v>0</v>
+      </c>
+      <c r="L3" s="11">
+        <v>1</v>
+      </c>
+      <c r="M3" s="11">
         <v>11</v>
       </c>
-      <c r="N3" s="14">
+      <c r="N3" s="11">
         <v>10</v>
       </c>
-      <c r="O3" s="14">
+      <c r="O3" s="11">
         <v>110</v>
       </c>
-      <c r="P3" s="14">
+      <c r="P3" s="11">
         <v>111</v>
       </c>
-      <c r="Q3" s="14">
+      <c r="Q3" s="11">
         <v>101</v>
       </c>
-      <c r="R3" s="15">
+      <c r="R3" s="12">
         <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A4" s="19">
-        <v>0</v>
-      </c>
-      <c r="B4" s="19">
-        <v>0</v>
-      </c>
-      <c r="C4" s="19">
-        <v>1</v>
-      </c>
-      <c r="D4" s="19">
-        <v>0</v>
-      </c>
-      <c r="E4" s="20">
-        <v>1</v>
-      </c>
-      <c r="F4" s="19">
-        <v>0</v>
-      </c>
-      <c r="G4" s="19">
-        <v>1</v>
-      </c>
-      <c r="H4" s="19">
-        <v>1</v>
-      </c>
-      <c r="J4" s="17">
-        <v>0</v>
-      </c>
-      <c r="K4" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="L4" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="M4" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="N4" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="O4" s="21" t="s">
-        <v>5</v>
-      </c>
-      <c r="P4" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="Q4" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="R4" s="22" t="s">
+      <c r="A4" s="16">
+        <v>0</v>
+      </c>
+      <c r="B4" s="16">
+        <v>0</v>
+      </c>
+      <c r="C4" s="16">
+        <v>1</v>
+      </c>
+      <c r="D4" s="16">
+        <v>0</v>
+      </c>
+      <c r="E4" s="17">
+        <v>1</v>
+      </c>
+      <c r="F4" s="16">
+        <v>0</v>
+      </c>
+      <c r="G4" s="16">
+        <v>1</v>
+      </c>
+      <c r="H4" s="16">
+        <v>1</v>
+      </c>
+      <c r="J4" s="14">
+        <v>0</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="L4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="M4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="N4" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="O4" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="P4" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q4" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="R4" s="19" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A5" s="19">
-        <v>0</v>
-      </c>
-      <c r="B5" s="19">
-        <v>1</v>
-      </c>
-      <c r="C5" s="19">
-        <v>0</v>
-      </c>
-      <c r="D5" s="19">
-        <v>0</v>
-      </c>
-      <c r="E5" s="20">
-        <v>1</v>
-      </c>
-      <c r="F5" s="19">
-        <v>0</v>
-      </c>
-      <c r="G5" s="19">
-        <v>1</v>
-      </c>
-      <c r="H5" s="19">
-        <v>1</v>
-      </c>
-      <c r="J5" s="17">
-        <v>1</v>
-      </c>
-      <c r="K5" s="8">
-        <v>0</v>
-      </c>
-      <c r="L5" s="8">
-        <v>0</v>
-      </c>
-      <c r="M5" s="8">
-        <v>1</v>
-      </c>
-      <c r="N5" s="8">
-        <v>0</v>
-      </c>
-      <c r="O5" s="8">
-        <v>1</v>
-      </c>
-      <c r="P5" s="8">
-        <v>0</v>
-      </c>
-      <c r="Q5" s="8">
-        <v>1</v>
-      </c>
-      <c r="R5" s="10">
+      <c r="A5" s="16">
+        <v>0</v>
+      </c>
+      <c r="B5" s="16">
+        <v>1</v>
+      </c>
+      <c r="C5" s="16">
+        <v>0</v>
+      </c>
+      <c r="D5" s="16">
+        <v>0</v>
+      </c>
+      <c r="E5" s="17">
+        <v>1</v>
+      </c>
+      <c r="F5" s="16">
+        <v>0</v>
+      </c>
+      <c r="G5" s="16">
+        <v>1</v>
+      </c>
+      <c r="H5" s="16">
+        <v>1</v>
+      </c>
+      <c r="J5" s="14">
+        <v>1</v>
+      </c>
+      <c r="K5" s="5">
+        <v>0</v>
+      </c>
+      <c r="L5" s="5">
+        <v>0</v>
+      </c>
+      <c r="M5" s="5">
+        <v>1</v>
+      </c>
+      <c r="N5" s="5">
+        <v>0</v>
+      </c>
+      <c r="O5" s="5">
+        <v>1</v>
+      </c>
+      <c r="P5" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="5">
+        <v>1</v>
+      </c>
+      <c r="R5" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A6" s="19">
-        <v>0</v>
-      </c>
-      <c r="B6" s="19">
-        <v>1</v>
-      </c>
-      <c r="C6" s="19">
-        <v>1</v>
-      </c>
-      <c r="D6" s="19">
-        <v>0</v>
-      </c>
-      <c r="E6" s="20">
-        <v>1</v>
-      </c>
-      <c r="F6" s="19">
-        <v>1</v>
-      </c>
-      <c r="G6" s="19">
-        <v>0</v>
-      </c>
-      <c r="H6" s="19">
-        <v>1</v>
-      </c>
-      <c r="J6" s="17">
+      <c r="A6" s="16">
+        <v>0</v>
+      </c>
+      <c r="B6" s="16">
+        <v>1</v>
+      </c>
+      <c r="C6" s="16">
+        <v>1</v>
+      </c>
+      <c r="D6" s="16">
+        <v>0</v>
+      </c>
+      <c r="E6" s="17">
+        <v>1</v>
+      </c>
+      <c r="F6" s="16">
+        <v>1</v>
+      </c>
+      <c r="G6" s="16">
+        <v>0</v>
+      </c>
+      <c r="H6" s="16">
+        <v>1</v>
+      </c>
+      <c r="J6" s="14">
         <v>11</v>
       </c>
-      <c r="K6" s="8">
-        <v>0</v>
-      </c>
-      <c r="L6" s="8">
-        <v>0</v>
-      </c>
-      <c r="M6" s="8">
-        <v>0</v>
-      </c>
-      <c r="N6" s="8">
-        <v>0</v>
-      </c>
-      <c r="O6" s="8">
-        <v>1</v>
-      </c>
-      <c r="P6" s="8">
-        <v>1</v>
-      </c>
-      <c r="Q6" s="8">
-        <v>1</v>
-      </c>
-      <c r="R6" s="10">
+      <c r="K6" s="5">
+        <v>0</v>
+      </c>
+      <c r="L6" s="5">
+        <v>0</v>
+      </c>
+      <c r="M6" s="5">
+        <v>0</v>
+      </c>
+      <c r="N6" s="5">
+        <v>0</v>
+      </c>
+      <c r="O6" s="5">
+        <v>1</v>
+      </c>
+      <c r="P6" s="5">
+        <v>1</v>
+      </c>
+      <c r="Q6" s="5">
+        <v>1</v>
+      </c>
+      <c r="R6" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A7" s="19">
-        <v>1</v>
-      </c>
-      <c r="B7" s="19">
-        <v>0</v>
-      </c>
-      <c r="C7" s="19">
-        <v>0</v>
-      </c>
-      <c r="D7" s="19">
-        <v>0</v>
-      </c>
-      <c r="E7" s="20">
-        <v>1</v>
-      </c>
-      <c r="F7" s="19">
-        <v>1</v>
-      </c>
-      <c r="G7" s="19">
-        <v>0</v>
-      </c>
-      <c r="H7" s="19">
-        <v>1</v>
-      </c>
-      <c r="J7" s="18">
+      <c r="A7" s="16">
+        <v>1</v>
+      </c>
+      <c r="B7" s="16">
+        <v>0</v>
+      </c>
+      <c r="C7" s="16">
+        <v>0</v>
+      </c>
+      <c r="D7" s="16">
+        <v>0</v>
+      </c>
+      <c r="E7" s="17">
+        <v>1</v>
+      </c>
+      <c r="F7" s="16">
+        <v>1</v>
+      </c>
+      <c r="G7" s="16">
+        <v>0</v>
+      </c>
+      <c r="H7" s="16">
+        <v>1</v>
+      </c>
+      <c r="J7" s="15">
         <v>10</v>
       </c>
-      <c r="K7" s="11">
-        <v>0</v>
-      </c>
-      <c r="L7" s="11">
-        <v>0</v>
-      </c>
-      <c r="M7" s="11">
-        <v>1</v>
-      </c>
-      <c r="N7" s="11">
-        <v>1</v>
-      </c>
-      <c r="O7" s="11">
-        <v>0</v>
-      </c>
-      <c r="P7" s="11">
-        <v>0</v>
-      </c>
-      <c r="Q7" s="11">
-        <v>1</v>
-      </c>
-      <c r="R7" s="12">
+      <c r="K7" s="8">
+        <v>0</v>
+      </c>
+      <c r="L7" s="8">
+        <v>0</v>
+      </c>
+      <c r="M7" s="8">
+        <v>1</v>
+      </c>
+      <c r="N7" s="8">
+        <v>1</v>
+      </c>
+      <c r="O7" s="8">
+        <v>0</v>
+      </c>
+      <c r="P7" s="8">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="8">
+        <v>1</v>
+      </c>
+      <c r="R7" s="9">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A8" s="19">
-        <v>1</v>
-      </c>
-      <c r="B8" s="19">
-        <v>0</v>
-      </c>
-      <c r="C8" s="19">
-        <v>1</v>
-      </c>
-      <c r="D8" s="19">
-        <v>0</v>
-      </c>
-      <c r="E8" s="20">
-        <v>1</v>
-      </c>
-      <c r="F8" s="19">
-        <v>1</v>
-      </c>
-      <c r="G8" s="19">
-        <v>1</v>
-      </c>
-      <c r="H8" s="19">
+      <c r="A8" s="16">
+        <v>1</v>
+      </c>
+      <c r="B8" s="16">
+        <v>0</v>
+      </c>
+      <c r="C8" s="16">
+        <v>1</v>
+      </c>
+      <c r="D8" s="16">
+        <v>0</v>
+      </c>
+      <c r="E8" s="17">
+        <v>1</v>
+      </c>
+      <c r="F8" s="16">
+        <v>1</v>
+      </c>
+      <c r="G8" s="16">
+        <v>1</v>
+      </c>
+      <c r="H8" s="16">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A9" s="19">
-        <v>1</v>
-      </c>
-      <c r="B9" s="19">
-        <v>1</v>
-      </c>
-      <c r="C9" s="19">
-        <v>0</v>
-      </c>
-      <c r="D9" s="19">
-        <v>0</v>
-      </c>
-      <c r="E9" s="20">
-        <v>1</v>
-      </c>
-      <c r="F9" s="19">
-        <v>1</v>
-      </c>
-      <c r="G9" s="19">
-        <v>1</v>
-      </c>
-      <c r="H9" s="19">
+      <c r="A9" s="16">
+        <v>1</v>
+      </c>
+      <c r="B9" s="16">
+        <v>1</v>
+      </c>
+      <c r="C9" s="16">
+        <v>0</v>
+      </c>
+      <c r="D9" s="16">
+        <v>0</v>
+      </c>
+      <c r="E9" s="17">
+        <v>1</v>
+      </c>
+      <c r="F9" s="16">
+        <v>1</v>
+      </c>
+      <c r="G9" s="16">
+        <v>1</v>
+      </c>
+      <c r="H9" s="16">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A10" s="19">
-        <v>1</v>
-      </c>
-      <c r="B10" s="19">
-        <v>1</v>
-      </c>
-      <c r="C10" s="19">
-        <v>1</v>
-      </c>
-      <c r="D10" s="19">
-        <v>0</v>
-      </c>
-      <c r="E10" s="20">
-        <v>1</v>
-      </c>
-      <c r="F10" s="19">
-        <v>0</v>
-      </c>
-      <c r="G10" s="19">
-        <v>0</v>
-      </c>
-      <c r="H10" s="19">
+      <c r="A10" s="16">
+        <v>1</v>
+      </c>
+      <c r="B10" s="16">
+        <v>1</v>
+      </c>
+      <c r="C10" s="16">
+        <v>1</v>
+      </c>
+      <c r="D10" s="16">
+        <v>0</v>
+      </c>
+      <c r="E10" s="17">
+        <v>1</v>
+      </c>
+      <c r="F10" s="16">
+        <v>0</v>
+      </c>
+      <c r="G10" s="16">
+        <v>0</v>
+      </c>
+      <c r="H10" s="16">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A11" s="19">
-        <v>0</v>
-      </c>
-      <c r="B11" s="19">
-        <v>0</v>
-      </c>
-      <c r="C11" s="19">
-        <v>0</v>
-      </c>
-      <c r="D11" s="19">
-        <v>1</v>
-      </c>
-      <c r="E11" s="20">
-        <v>0</v>
-      </c>
-      <c r="F11" s="19">
-        <v>0</v>
-      </c>
-      <c r="G11" s="19">
-        <v>1</v>
-      </c>
-      <c r="H11" s="19">
-        <v>0</v>
-      </c>
-      <c r="J11" s="13" t="s">
+      <c r="A11" s="16">
+        <v>0</v>
+      </c>
+      <c r="B11" s="16">
+        <v>0</v>
+      </c>
+      <c r="C11" s="16">
+        <v>0</v>
+      </c>
+      <c r="D11" s="16">
+        <v>1</v>
+      </c>
+      <c r="E11" s="17">
+        <v>0</v>
+      </c>
+      <c r="F11" s="16">
+        <v>0</v>
+      </c>
+      <c r="G11" s="16">
+        <v>1</v>
+      </c>
+      <c r="H11" s="16">
+        <v>0</v>
+      </c>
+      <c r="J11" s="10" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A12" s="19">
-        <v>0</v>
-      </c>
-      <c r="B12" s="19">
-        <v>0</v>
-      </c>
-      <c r="C12" s="19">
-        <v>1</v>
-      </c>
-      <c r="D12" s="19">
-        <v>1</v>
-      </c>
-      <c r="E12" s="20">
-        <v>0</v>
-      </c>
-      <c r="F12" s="19">
-        <v>0</v>
-      </c>
-      <c r="G12" s="19">
-        <v>1</v>
-      </c>
-      <c r="H12" s="19">
-        <v>0</v>
-      </c>
-      <c r="J12" s="16"/>
-      <c r="K12" s="14">
-        <v>0</v>
-      </c>
-      <c r="L12" s="14">
-        <v>1</v>
-      </c>
-      <c r="M12" s="14">
+      <c r="A12" s="16">
+        <v>0</v>
+      </c>
+      <c r="B12" s="16">
+        <v>0</v>
+      </c>
+      <c r="C12" s="16">
+        <v>1</v>
+      </c>
+      <c r="D12" s="16">
+        <v>1</v>
+      </c>
+      <c r="E12" s="17">
+        <v>0</v>
+      </c>
+      <c r="F12" s="16">
+        <v>0</v>
+      </c>
+      <c r="G12" s="16">
+        <v>1</v>
+      </c>
+      <c r="H12" s="16">
+        <v>0</v>
+      </c>
+      <c r="J12" s="13"/>
+      <c r="K12" s="11">
+        <v>0</v>
+      </c>
+      <c r="L12" s="11">
+        <v>1</v>
+      </c>
+      <c r="M12" s="11">
         <v>11</v>
       </c>
-      <c r="N12" s="14">
+      <c r="N12" s="11">
         <v>10</v>
       </c>
-      <c r="O12" s="14">
+      <c r="O12" s="11">
         <v>110</v>
       </c>
-      <c r="P12" s="14">
+      <c r="P12" s="11">
         <v>111</v>
       </c>
-      <c r="Q12" s="14">
+      <c r="Q12" s="11">
         <v>101</v>
       </c>
-      <c r="R12" s="15">
+      <c r="R12" s="12">
         <v>100</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A13" s="19">
-        <v>0</v>
-      </c>
-      <c r="B13" s="19">
-        <v>1</v>
-      </c>
-      <c r="C13" s="19">
-        <v>0</v>
-      </c>
-      <c r="D13" s="19">
-        <v>1</v>
-      </c>
-      <c r="E13" s="20">
-        <v>0</v>
-      </c>
-      <c r="F13" s="19">
-        <v>1</v>
-      </c>
-      <c r="G13" s="19">
-        <v>0</v>
-      </c>
-      <c r="H13" s="19">
-        <v>0</v>
-      </c>
-      <c r="J13" s="17">
-        <v>0</v>
-      </c>
-      <c r="K13" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="L13" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="M13" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="N13" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="O13" s="21" t="s">
-        <v>5</v>
-      </c>
-      <c r="P13" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="Q13" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="R13" s="22" t="s">
+      <c r="A13" s="16">
+        <v>0</v>
+      </c>
+      <c r="B13" s="16">
+        <v>1</v>
+      </c>
+      <c r="C13" s="16">
+        <v>0</v>
+      </c>
+      <c r="D13" s="16">
+        <v>1</v>
+      </c>
+      <c r="E13" s="17">
+        <v>0</v>
+      </c>
+      <c r="F13" s="16">
+        <v>1</v>
+      </c>
+      <c r="G13" s="16">
+        <v>0</v>
+      </c>
+      <c r="H13" s="16">
+        <v>0</v>
+      </c>
+      <c r="J13" s="14">
+        <v>0</v>
+      </c>
+      <c r="K13" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="L13" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="M13" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="N13" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="O13" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="P13" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q13" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="R13" s="19" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A14" s="19">
-        <v>0</v>
-      </c>
-      <c r="B14" s="19">
-        <v>1</v>
-      </c>
-      <c r="C14" s="19">
-        <v>1</v>
-      </c>
-      <c r="D14" s="19">
-        <v>1</v>
-      </c>
-      <c r="E14" s="20">
-        <v>0</v>
-      </c>
-      <c r="F14" s="19">
-        <v>1</v>
-      </c>
-      <c r="G14" s="19">
-        <v>0</v>
-      </c>
-      <c r="H14" s="19">
-        <v>0</v>
-      </c>
-      <c r="J14" s="17">
-        <v>1</v>
-      </c>
-      <c r="K14" s="8">
-        <v>0</v>
-      </c>
-      <c r="L14" s="8">
-        <v>1</v>
-      </c>
-      <c r="M14" s="8">
-        <v>0</v>
-      </c>
-      <c r="N14" s="8">
-        <v>1</v>
-      </c>
-      <c r="O14" s="8">
-        <v>1</v>
-      </c>
-      <c r="P14" s="8">
-        <v>0</v>
-      </c>
-      <c r="Q14" s="8">
-        <v>1</v>
-      </c>
-      <c r="R14" s="10">
+      <c r="A14" s="16">
+        <v>0</v>
+      </c>
+      <c r="B14" s="16">
+        <v>1</v>
+      </c>
+      <c r="C14" s="16">
+        <v>1</v>
+      </c>
+      <c r="D14" s="16">
+        <v>1</v>
+      </c>
+      <c r="E14" s="17">
+        <v>0</v>
+      </c>
+      <c r="F14" s="16">
+        <v>1</v>
+      </c>
+      <c r="G14" s="16">
+        <v>0</v>
+      </c>
+      <c r="H14" s="16">
+        <v>0</v>
+      </c>
+      <c r="J14" s="14">
+        <v>1</v>
+      </c>
+      <c r="K14" s="5">
+        <v>0</v>
+      </c>
+      <c r="L14" s="5">
+        <v>1</v>
+      </c>
+      <c r="M14" s="5">
+        <v>0</v>
+      </c>
+      <c r="N14" s="5">
+        <v>1</v>
+      </c>
+      <c r="O14" s="5">
+        <v>1</v>
+      </c>
+      <c r="P14" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="5">
+        <v>1</v>
+      </c>
+      <c r="R14" s="7">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A15" s="19">
-        <v>1</v>
-      </c>
-      <c r="B15" s="19">
-        <v>0</v>
-      </c>
-      <c r="C15" s="19">
-        <v>0</v>
-      </c>
-      <c r="D15" s="19">
-        <v>1</v>
-      </c>
-      <c r="E15" s="20">
-        <v>0</v>
-      </c>
-      <c r="F15" s="19">
-        <v>1</v>
-      </c>
-      <c r="G15" s="19">
-        <v>1</v>
-      </c>
-      <c r="H15" s="19">
-        <v>0</v>
-      </c>
-      <c r="J15" s="17">
+      <c r="A15" s="16">
+        <v>1</v>
+      </c>
+      <c r="B15" s="16">
+        <v>0</v>
+      </c>
+      <c r="C15" s="16">
+        <v>0</v>
+      </c>
+      <c r="D15" s="16">
+        <v>1</v>
+      </c>
+      <c r="E15" s="17">
+        <v>0</v>
+      </c>
+      <c r="F15" s="16">
+        <v>1</v>
+      </c>
+      <c r="G15" s="16">
+        <v>1</v>
+      </c>
+      <c r="H15" s="16">
+        <v>0</v>
+      </c>
+      <c r="J15" s="14">
         <v>11</v>
       </c>
-      <c r="K15" s="8">
-        <v>0</v>
-      </c>
-      <c r="L15" s="8">
-        <v>0</v>
-      </c>
-      <c r="M15" s="8">
-        <v>1</v>
-      </c>
-      <c r="N15" s="8">
-        <v>1</v>
-      </c>
-      <c r="O15" s="8">
-        <v>1</v>
-      </c>
-      <c r="P15" s="8">
-        <v>1</v>
-      </c>
-      <c r="Q15" s="8">
-        <v>0</v>
-      </c>
-      <c r="R15" s="10">
+      <c r="K15" s="5">
+        <v>0</v>
+      </c>
+      <c r="L15" s="5">
+        <v>0</v>
+      </c>
+      <c r="M15" s="5">
+        <v>1</v>
+      </c>
+      <c r="N15" s="5">
+        <v>1</v>
+      </c>
+      <c r="O15" s="5">
+        <v>1</v>
+      </c>
+      <c r="P15" s="5">
+        <v>1</v>
+      </c>
+      <c r="Q15" s="5">
+        <v>0</v>
+      </c>
+      <c r="R15" s="7">
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A16" s="19">
-        <v>1</v>
-      </c>
-      <c r="B16" s="19">
-        <v>0</v>
-      </c>
-      <c r="C16" s="19">
-        <v>1</v>
-      </c>
-      <c r="D16" s="19">
-        <v>1</v>
-      </c>
-      <c r="E16" s="20">
-        <v>0</v>
-      </c>
-      <c r="F16" s="19">
-        <v>1</v>
-      </c>
-      <c r="G16" s="19">
-        <v>1</v>
-      </c>
-      <c r="H16" s="19">
-        <v>0</v>
-      </c>
-      <c r="J16" s="18">
+      <c r="A16" s="16">
+        <v>1</v>
+      </c>
+      <c r="B16" s="16">
+        <v>0</v>
+      </c>
+      <c r="C16" s="16">
+        <v>1</v>
+      </c>
+      <c r="D16" s="16">
+        <v>1</v>
+      </c>
+      <c r="E16" s="17">
+        <v>0</v>
+      </c>
+      <c r="F16" s="16">
+        <v>1</v>
+      </c>
+      <c r="G16" s="16">
+        <v>1</v>
+      </c>
+      <c r="H16" s="16">
+        <v>0</v>
+      </c>
+      <c r="J16" s="15">
         <v>10</v>
       </c>
-      <c r="K16" s="11">
-        <v>1</v>
-      </c>
-      <c r="L16" s="11">
-        <v>1</v>
-      </c>
-      <c r="M16" s="11">
-        <v>0</v>
-      </c>
-      <c r="N16" s="11">
-        <v>0</v>
-      </c>
-      <c r="O16" s="11">
-        <v>0</v>
-      </c>
-      <c r="P16" s="11">
-        <v>0</v>
-      </c>
-      <c r="Q16" s="11">
-        <v>1</v>
-      </c>
-      <c r="R16" s="12">
+      <c r="K16" s="8">
+        <v>1</v>
+      </c>
+      <c r="L16" s="8">
+        <v>1</v>
+      </c>
+      <c r="M16" s="8">
+        <v>0</v>
+      </c>
+      <c r="N16" s="8">
+        <v>0</v>
+      </c>
+      <c r="O16" s="8">
+        <v>0</v>
+      </c>
+      <c r="P16" s="8">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="8">
+        <v>1</v>
+      </c>
+      <c r="R16" s="9">
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A17" s="19">
-        <v>1</v>
-      </c>
-      <c r="B17" s="19">
-        <v>1</v>
-      </c>
-      <c r="C17" s="19">
-        <v>0</v>
-      </c>
-      <c r="D17" s="19">
-        <v>1</v>
-      </c>
-      <c r="E17" s="20">
-        <v>0</v>
-      </c>
-      <c r="F17" s="19">
-        <v>0</v>
-      </c>
-      <c r="G17" s="19">
-        <v>0</v>
-      </c>
-      <c r="H17" s="19">
+      <c r="A17" s="16">
+        <v>1</v>
+      </c>
+      <c r="B17" s="16">
+        <v>1</v>
+      </c>
+      <c r="C17" s="16">
+        <v>0</v>
+      </c>
+      <c r="D17" s="16">
+        <v>1</v>
+      </c>
+      <c r="E17" s="17">
+        <v>0</v>
+      </c>
+      <c r="F17" s="16">
+        <v>0</v>
+      </c>
+      <c r="G17" s="16">
+        <v>0</v>
+      </c>
+      <c r="H17" s="16">
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A18" s="19">
-        <v>1</v>
-      </c>
-      <c r="B18" s="19">
-        <v>1</v>
-      </c>
-      <c r="C18" s="19">
-        <v>1</v>
-      </c>
-      <c r="D18" s="19">
-        <v>1</v>
-      </c>
-      <c r="E18" s="20">
-        <v>0</v>
-      </c>
-      <c r="F18" s="19">
-        <v>0</v>
-      </c>
-      <c r="G18" s="19">
-        <v>0</v>
-      </c>
-      <c r="H18" s="19">
+      <c r="A18" s="16">
+        <v>1</v>
+      </c>
+      <c r="B18" s="16">
+        <v>1</v>
+      </c>
+      <c r="C18" s="16">
+        <v>1</v>
+      </c>
+      <c r="D18" s="16">
+        <v>1</v>
+      </c>
+      <c r="E18" s="17">
+        <v>0</v>
+      </c>
+      <c r="F18" s="16">
+        <v>0</v>
+      </c>
+      <c r="G18" s="16">
+        <v>0</v>
+      </c>
+      <c r="H18" s="16">
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A19" s="19">
-        <v>0</v>
-      </c>
-      <c r="B19" s="19">
-        <v>0</v>
-      </c>
-      <c r="C19" s="19">
-        <v>0</v>
-      </c>
-      <c r="D19" s="19">
-        <v>1</v>
-      </c>
-      <c r="E19" s="20">
-        <v>1</v>
-      </c>
-      <c r="F19" s="19">
-        <v>0</v>
-      </c>
-      <c r="G19" s="19">
-        <v>0</v>
-      </c>
-      <c r="H19" s="19">
+      <c r="A19" s="16">
+        <v>0</v>
+      </c>
+      <c r="B19" s="16">
+        <v>0</v>
+      </c>
+      <c r="C19" s="16">
+        <v>0</v>
+      </c>
+      <c r="D19" s="16">
+        <v>1</v>
+      </c>
+      <c r="E19" s="17">
+        <v>1</v>
+      </c>
+      <c r="F19" s="16">
+        <v>0</v>
+      </c>
+      <c r="G19" s="16">
+        <v>0</v>
+      </c>
+      <c r="H19" s="16">
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A20" s="19">
-        <v>0</v>
-      </c>
-      <c r="B20" s="19">
-        <v>0</v>
-      </c>
-      <c r="C20" s="19">
-        <v>1</v>
-      </c>
-      <c r="D20" s="19">
-        <v>1</v>
-      </c>
-      <c r="E20" s="20">
-        <v>1</v>
-      </c>
-      <c r="F20" s="19">
-        <v>0</v>
-      </c>
-      <c r="G20" s="19">
-        <v>0</v>
-      </c>
-      <c r="H20" s="19">
-        <v>1</v>
-      </c>
-      <c r="J20" s="13" t="s">
+      <c r="A20" s="16">
+        <v>0</v>
+      </c>
+      <c r="B20" s="16">
+        <v>0</v>
+      </c>
+      <c r="C20" s="16">
+        <v>1</v>
+      </c>
+      <c r="D20" s="16">
+        <v>1</v>
+      </c>
+      <c r="E20" s="17">
+        <v>1</v>
+      </c>
+      <c r="F20" s="16">
+        <v>0</v>
+      </c>
+      <c r="G20" s="16">
+        <v>0</v>
+      </c>
+      <c r="H20" s="16">
+        <v>1</v>
+      </c>
+      <c r="J20" s="10" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A21" s="19">
-        <v>0</v>
-      </c>
-      <c r="B21" s="19">
-        <v>1</v>
-      </c>
-      <c r="C21" s="19">
-        <v>0</v>
-      </c>
-      <c r="D21" s="19">
-        <v>1</v>
-      </c>
-      <c r="E21" s="20">
-        <v>1</v>
-      </c>
-      <c r="F21" s="19">
-        <v>0</v>
-      </c>
-      <c r="G21" s="19">
-        <v>1</v>
-      </c>
-      <c r="H21" s="19">
-        <v>0</v>
-      </c>
-      <c r="J21" s="16"/>
-      <c r="K21" s="14">
-        <v>0</v>
-      </c>
-      <c r="L21" s="14">
-        <v>1</v>
-      </c>
-      <c r="M21" s="14">
+      <c r="A21" s="16">
+        <v>0</v>
+      </c>
+      <c r="B21" s="16">
+        <v>1</v>
+      </c>
+      <c r="C21" s="16">
+        <v>0</v>
+      </c>
+      <c r="D21" s="16">
+        <v>1</v>
+      </c>
+      <c r="E21" s="17">
+        <v>1</v>
+      </c>
+      <c r="F21" s="16">
+        <v>0</v>
+      </c>
+      <c r="G21" s="16">
+        <v>1</v>
+      </c>
+      <c r="H21" s="16">
+        <v>0</v>
+      </c>
+      <c r="J21" s="13"/>
+      <c r="K21" s="11">
+        <v>0</v>
+      </c>
+      <c r="L21" s="11">
+        <v>1</v>
+      </c>
+      <c r="M21" s="11">
         <v>11</v>
       </c>
-      <c r="N21" s="14">
+      <c r="N21" s="11">
         <v>10</v>
       </c>
-      <c r="O21" s="14">
+      <c r="O21" s="11">
         <v>110</v>
       </c>
-      <c r="P21" s="14">
+      <c r="P21" s="11">
         <v>111</v>
       </c>
-      <c r="Q21" s="14">
+      <c r="Q21" s="11">
         <v>101</v>
       </c>
-      <c r="R21" s="15">
+      <c r="R21" s="12">
         <v>100</v>
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A22" s="19">
-        <v>0</v>
-      </c>
-      <c r="B22" s="19">
-        <v>1</v>
-      </c>
-      <c r="C22" s="19">
-        <v>1</v>
-      </c>
-      <c r="D22" s="19">
-        <v>1</v>
-      </c>
-      <c r="E22" s="20">
-        <v>1</v>
-      </c>
-      <c r="F22" s="19">
-        <v>0</v>
-      </c>
-      <c r="G22" s="19">
-        <v>1</v>
-      </c>
-      <c r="H22" s="19">
-        <v>1</v>
-      </c>
-      <c r="J22" s="17">
-        <v>0</v>
-      </c>
-      <c r="K22" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="L22" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="M22" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="N22" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="O22" s="21" t="s">
-        <v>5</v>
-      </c>
-      <c r="P22" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="Q22" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="R22" s="22" t="s">
+      <c r="A22" s="16">
+        <v>0</v>
+      </c>
+      <c r="B22" s="16">
+        <v>1</v>
+      </c>
+      <c r="C22" s="16">
+        <v>1</v>
+      </c>
+      <c r="D22" s="16">
+        <v>1</v>
+      </c>
+      <c r="E22" s="17">
+        <v>1</v>
+      </c>
+      <c r="F22" s="16">
+        <v>0</v>
+      </c>
+      <c r="G22" s="16">
+        <v>1</v>
+      </c>
+      <c r="H22" s="16">
+        <v>1</v>
+      </c>
+      <c r="J22" s="14">
+        <v>0</v>
+      </c>
+      <c r="K22" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="L22" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="M22" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="N22" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="O22" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="P22" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q22" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="R22" s="19" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A23" s="19">
-        <v>1</v>
-      </c>
-      <c r="B23" s="19">
-        <v>0</v>
-      </c>
-      <c r="C23" s="19">
-        <v>0</v>
-      </c>
-      <c r="D23" s="19">
-        <v>1</v>
-      </c>
-      <c r="E23" s="20">
-        <v>1</v>
-      </c>
-      <c r="F23" s="19">
-        <v>1</v>
-      </c>
-      <c r="G23" s="19">
-        <v>0</v>
-      </c>
-      <c r="H23" s="19">
-        <v>0</v>
-      </c>
-      <c r="J23" s="17">
-        <v>1</v>
-      </c>
-      <c r="K23" s="8">
-        <v>1</v>
-      </c>
-      <c r="L23" s="8">
-        <v>1</v>
-      </c>
-      <c r="M23" s="8">
-        <v>1</v>
-      </c>
-      <c r="N23" s="8">
-        <v>1</v>
-      </c>
-      <c r="O23" s="8">
-        <v>1</v>
-      </c>
-      <c r="P23" s="8">
-        <v>1</v>
-      </c>
-      <c r="Q23" s="8">
-        <v>1</v>
-      </c>
-      <c r="R23" s="10">
+      <c r="A23" s="16">
+        <v>1</v>
+      </c>
+      <c r="B23" s="16">
+        <v>0</v>
+      </c>
+      <c r="C23" s="16">
+        <v>0</v>
+      </c>
+      <c r="D23" s="16">
+        <v>1</v>
+      </c>
+      <c r="E23" s="17">
+        <v>1</v>
+      </c>
+      <c r="F23" s="16">
+        <v>1</v>
+      </c>
+      <c r="G23" s="16">
+        <v>0</v>
+      </c>
+      <c r="H23" s="16">
+        <v>0</v>
+      </c>
+      <c r="J23" s="14">
+        <v>1</v>
+      </c>
+      <c r="K23" s="5">
+        <v>1</v>
+      </c>
+      <c r="L23" s="5">
+        <v>1</v>
+      </c>
+      <c r="M23" s="5">
+        <v>1</v>
+      </c>
+      <c r="N23" s="5">
+        <v>1</v>
+      </c>
+      <c r="O23" s="5">
+        <v>1</v>
+      </c>
+      <c r="P23" s="5">
+        <v>1</v>
+      </c>
+      <c r="Q23" s="5">
+        <v>1</v>
+      </c>
+      <c r="R23" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A24" s="19">
-        <v>1</v>
-      </c>
-      <c r="B24" s="19">
-        <v>0</v>
-      </c>
-      <c r="C24" s="19">
-        <v>1</v>
-      </c>
-      <c r="D24" s="19">
-        <v>1</v>
-      </c>
-      <c r="E24" s="20">
-        <v>1</v>
-      </c>
-      <c r="F24" s="19">
-        <v>1</v>
-      </c>
-      <c r="G24" s="19">
-        <v>0</v>
-      </c>
-      <c r="H24" s="19">
-        <v>1</v>
-      </c>
-      <c r="J24" s="17">
+      <c r="A24" s="16">
+        <v>1</v>
+      </c>
+      <c r="B24" s="16">
+        <v>0</v>
+      </c>
+      <c r="C24" s="16">
+        <v>1</v>
+      </c>
+      <c r="D24" s="16">
+        <v>1</v>
+      </c>
+      <c r="E24" s="17">
+        <v>1</v>
+      </c>
+      <c r="F24" s="16">
+        <v>1</v>
+      </c>
+      <c r="G24" s="16">
+        <v>0</v>
+      </c>
+      <c r="H24" s="16">
+        <v>1</v>
+      </c>
+      <c r="J24" s="14">
         <v>11</v>
       </c>
-      <c r="K24" s="8">
-        <v>0</v>
-      </c>
-      <c r="L24" s="8">
-        <v>1</v>
-      </c>
-      <c r="M24" s="8">
-        <v>1</v>
-      </c>
-      <c r="N24" s="8">
-        <v>0</v>
-      </c>
-      <c r="O24" s="8">
-        <v>0</v>
-      </c>
-      <c r="P24" s="8">
-        <v>1</v>
-      </c>
-      <c r="Q24" s="8">
-        <v>1</v>
-      </c>
-      <c r="R24" s="10">
+      <c r="K24" s="5">
+        <v>0</v>
+      </c>
+      <c r="L24" s="5">
+        <v>1</v>
+      </c>
+      <c r="M24" s="5">
+        <v>1</v>
+      </c>
+      <c r="N24" s="5">
+        <v>0</v>
+      </c>
+      <c r="O24" s="5">
+        <v>0</v>
+      </c>
+      <c r="P24" s="5">
+        <v>1</v>
+      </c>
+      <c r="Q24" s="5">
+        <v>1</v>
+      </c>
+      <c r="R24" s="7">
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A25" s="19">
-        <v>1</v>
-      </c>
-      <c r="B25" s="19">
-        <v>1</v>
-      </c>
-      <c r="C25" s="19">
-        <v>0</v>
-      </c>
-      <c r="D25" s="19">
-        <v>1</v>
-      </c>
-      <c r="E25" s="20">
-        <v>1</v>
-      </c>
-      <c r="F25" s="19">
-        <v>1</v>
-      </c>
-      <c r="G25" s="19">
-        <v>1</v>
-      </c>
-      <c r="H25" s="19">
-        <v>0</v>
-      </c>
-      <c r="J25" s="18">
+      <c r="A25" s="16">
+        <v>1</v>
+      </c>
+      <c r="B25" s="16">
+        <v>1</v>
+      </c>
+      <c r="C25" s="16">
+        <v>0</v>
+      </c>
+      <c r="D25" s="16">
+        <v>1</v>
+      </c>
+      <c r="E25" s="17">
+        <v>1</v>
+      </c>
+      <c r="F25" s="16">
+        <v>1</v>
+      </c>
+      <c r="G25" s="16">
+        <v>1</v>
+      </c>
+      <c r="H25" s="16">
+        <v>0</v>
+      </c>
+      <c r="J25" s="15">
         <v>10</v>
       </c>
-      <c r="K25" s="11">
-        <v>0</v>
-      </c>
-      <c r="L25" s="11">
-        <v>0</v>
-      </c>
-      <c r="M25" s="11">
-        <v>0</v>
-      </c>
-      <c r="N25" s="11">
-        <v>0</v>
-      </c>
-      <c r="O25" s="11">
-        <v>0</v>
-      </c>
-      <c r="P25" s="11">
-        <v>0</v>
-      </c>
-      <c r="Q25" s="11">
-        <v>0</v>
-      </c>
-      <c r="R25" s="12">
+      <c r="K25" s="8">
+        <v>0</v>
+      </c>
+      <c r="L25" s="8">
+        <v>0</v>
+      </c>
+      <c r="M25" s="8">
+        <v>0</v>
+      </c>
+      <c r="N25" s="8">
+        <v>0</v>
+      </c>
+      <c r="O25" s="8">
+        <v>0</v>
+      </c>
+      <c r="P25" s="8">
+        <v>0</v>
+      </c>
+      <c r="Q25" s="8">
+        <v>0</v>
+      </c>
+      <c r="R25" s="9">
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A26" s="19">
-        <v>1</v>
-      </c>
-      <c r="B26" s="19">
-        <v>1</v>
-      </c>
-      <c r="C26" s="19">
-        <v>1</v>
-      </c>
-      <c r="D26" s="19">
-        <v>1</v>
-      </c>
-      <c r="E26" s="20">
-        <v>1</v>
-      </c>
-      <c r="F26" s="19">
-        <v>1</v>
-      </c>
-      <c r="G26" s="19">
-        <v>1</v>
-      </c>
-      <c r="H26" s="19">
+      <c r="A26" s="16">
+        <v>1</v>
+      </c>
+      <c r="B26" s="16">
+        <v>1</v>
+      </c>
+      <c r="C26" s="16">
+        <v>1</v>
+      </c>
+      <c r="D26" s="16">
+        <v>1</v>
+      </c>
+      <c r="E26" s="17">
+        <v>1</v>
+      </c>
+      <c r="F26" s="16">
+        <v>1</v>
+      </c>
+      <c r="G26" s="16">
+        <v>1</v>
+      </c>
+      <c r="H26" s="16">
         <v>1</v>
       </c>
     </row>
@@ -3153,86 +3177,1540 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O6"/>
+  <dimension ref="A1:AB26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:J6"/>
+      <selection activeCell="Q10" sqref="Q10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="3" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="2.7109375" customWidth="1"/>
+    <col min="6" max="8" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="18" width="9.140625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C2" s="5">
-        <v>0</v>
-      </c>
-      <c r="D2" s="5">
-        <v>1</v>
-      </c>
-      <c r="E2" s="5">
+    <row r="1" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A2" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="16">
+        <v>0</v>
+      </c>
+      <c r="E2" s="17">
+        <v>0</v>
+      </c>
+      <c r="F2" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" s="21"/>
+      <c r="J2" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="T2" s="10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A3" s="16">
+        <v>0</v>
+      </c>
+      <c r="B3" s="16">
+        <v>0</v>
+      </c>
+      <c r="C3" s="20">
+        <v>0</v>
+      </c>
+      <c r="D3" s="16">
+        <v>0</v>
+      </c>
+      <c r="E3" s="17">
+        <v>1</v>
+      </c>
+      <c r="F3" s="16">
+        <v>0</v>
+      </c>
+      <c r="G3" s="16">
+        <v>0</v>
+      </c>
+      <c r="H3" s="20">
+        <v>1</v>
+      </c>
+      <c r="I3" s="21"/>
+      <c r="J3" s="13"/>
+      <c r="K3" s="11">
+        <v>0</v>
+      </c>
+      <c r="L3" s="11">
+        <v>1</v>
+      </c>
+      <c r="M3" s="11">
         <v>11</v>
       </c>
-      <c r="F2" s="5">
+      <c r="N3" s="11">
         <v>10</v>
       </c>
-      <c r="G2" s="5">
+      <c r="O3" s="11">
+        <v>110</v>
+      </c>
+      <c r="P3" s="11">
+        <v>111</v>
+      </c>
+      <c r="Q3" s="11">
+        <v>101</v>
+      </c>
+      <c r="R3" s="12">
         <v>100</v>
       </c>
-      <c r="H2" s="5">
+      <c r="T3" s="13"/>
+      <c r="U3" s="11">
+        <v>0</v>
+      </c>
+      <c r="V3" s="11">
+        <v>1</v>
+      </c>
+      <c r="W3" s="11">
+        <v>11</v>
+      </c>
+      <c r="X3" s="11">
+        <v>10</v>
+      </c>
+      <c r="Y3" s="11">
+        <v>110</v>
+      </c>
+      <c r="Z3" s="11">
+        <v>111</v>
+      </c>
+      <c r="AA3" s="11">
         <v>101</v>
       </c>
-      <c r="I2" s="5">
+      <c r="AB3" s="12">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A4" s="16">
+        <v>0</v>
+      </c>
+      <c r="B4" s="16">
+        <v>0</v>
+      </c>
+      <c r="C4" s="20">
+        <v>1</v>
+      </c>
+      <c r="D4" s="16">
+        <v>0</v>
+      </c>
+      <c r="E4" s="17">
+        <v>1</v>
+      </c>
+      <c r="F4" s="16">
+        <v>0</v>
+      </c>
+      <c r="G4" s="16">
+        <v>1</v>
+      </c>
+      <c r="H4" s="20">
+        <v>1</v>
+      </c>
+      <c r="I4" s="21"/>
+      <c r="J4" s="14">
+        <v>0</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="L4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="M4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="N4" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="O4" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="P4" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q4" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="R4" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="T4" s="14">
+        <v>0</v>
+      </c>
+      <c r="U4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="V4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="W4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="X4" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="Y4" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z4" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="AA4" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="AB4" s="19" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A5" s="16">
+        <v>0</v>
+      </c>
+      <c r="B5" s="16">
+        <v>1</v>
+      </c>
+      <c r="C5" s="20">
+        <v>0</v>
+      </c>
+      <c r="D5" s="16">
+        <v>0</v>
+      </c>
+      <c r="E5" s="17">
+        <v>1</v>
+      </c>
+      <c r="F5" s="16">
+        <v>0</v>
+      </c>
+      <c r="G5" s="16">
+        <v>1</v>
+      </c>
+      <c r="H5" s="20">
+        <v>1</v>
+      </c>
+      <c r="I5" s="21"/>
+      <c r="J5" s="14">
+        <v>1</v>
+      </c>
+      <c r="K5" s="5">
+        <v>0</v>
+      </c>
+      <c r="L5" s="5">
+        <v>0</v>
+      </c>
+      <c r="M5" s="5">
+        <v>1</v>
+      </c>
+      <c r="N5" s="5">
+        <v>0</v>
+      </c>
+      <c r="O5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="P5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="R5" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="T5" s="14">
+        <v>1</v>
+      </c>
+      <c r="U5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="V5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="W5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="X5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="Y5" s="5">
+        <v>0</v>
+      </c>
+      <c r="Z5" s="5">
+        <v>1</v>
+      </c>
+      <c r="AA5" s="5">
+        <v>0</v>
+      </c>
+      <c r="AB5" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A6" s="16">
+        <v>0</v>
+      </c>
+      <c r="B6" s="16">
+        <v>1</v>
+      </c>
+      <c r="C6" s="20">
+        <v>1</v>
+      </c>
+      <c r="D6" s="16">
+        <v>0</v>
+      </c>
+      <c r="E6" s="17">
+        <v>1</v>
+      </c>
+      <c r="F6" s="16">
+        <v>1</v>
+      </c>
+      <c r="G6" s="16">
+        <v>0</v>
+      </c>
+      <c r="H6" s="20">
+        <v>1</v>
+      </c>
+      <c r="I6" s="21"/>
+      <c r="J6" s="14">
+        <v>11</v>
+      </c>
+      <c r="K6" s="5">
+        <v>0</v>
+      </c>
+      <c r="L6" s="5">
+        <v>0</v>
+      </c>
+      <c r="M6" s="5">
+        <v>0</v>
+      </c>
+      <c r="N6" s="5">
+        <v>0</v>
+      </c>
+      <c r="O6" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="P6" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q6" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="R6" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="T6" s="14">
+        <v>11</v>
+      </c>
+      <c r="U6" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="V6" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="W6" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="X6" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="Y6" s="5">
+        <v>0</v>
+      </c>
+      <c r="Z6" s="5">
+        <v>0</v>
+      </c>
+      <c r="AA6" s="5">
+        <v>0</v>
+      </c>
+      <c r="AB6" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A7" s="16">
+        <v>1</v>
+      </c>
+      <c r="B7" s="16">
+        <v>0</v>
+      </c>
+      <c r="C7" s="20">
+        <v>0</v>
+      </c>
+      <c r="D7" s="16">
+        <v>0</v>
+      </c>
+      <c r="E7" s="17">
+        <v>1</v>
+      </c>
+      <c r="F7" s="16">
+        <v>1</v>
+      </c>
+      <c r="G7" s="16">
+        <v>0</v>
+      </c>
+      <c r="H7" s="20">
+        <v>1</v>
+      </c>
+      <c r="I7" s="21"/>
+      <c r="J7" s="15">
+        <v>10</v>
+      </c>
+      <c r="K7" s="8">
+        <v>0</v>
+      </c>
+      <c r="L7" s="8">
+        <v>0</v>
+      </c>
+      <c r="M7" s="8">
+        <v>1</v>
+      </c>
+      <c r="N7" s="8">
+        <v>1</v>
+      </c>
+      <c r="O7" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="P7" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q7" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="R7" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="T7" s="15">
+        <v>10</v>
+      </c>
+      <c r="U7" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="V7" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="W7" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="X7" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="Y7" s="8">
+        <v>1</v>
+      </c>
+      <c r="Z7" s="8">
+        <v>1</v>
+      </c>
+      <c r="AA7" s="8">
+        <v>0</v>
+      </c>
+      <c r="AB7" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A8" s="16">
+        <v>1</v>
+      </c>
+      <c r="B8" s="16">
+        <v>0</v>
+      </c>
+      <c r="C8" s="20">
+        <v>1</v>
+      </c>
+      <c r="D8" s="16">
+        <v>0</v>
+      </c>
+      <c r="E8" s="17">
+        <v>1</v>
+      </c>
+      <c r="F8" s="16">
+        <v>1</v>
+      </c>
+      <c r="G8" s="16">
+        <v>1</v>
+      </c>
+      <c r="H8" s="20">
+        <v>1</v>
+      </c>
+      <c r="I8" s="21"/>
+    </row>
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A9" s="16">
+        <v>1</v>
+      </c>
+      <c r="B9" s="16">
+        <v>1</v>
+      </c>
+      <c r="C9" s="20">
+        <v>0</v>
+      </c>
+      <c r="D9" s="16">
+        <v>0</v>
+      </c>
+      <c r="E9" s="17">
+        <v>1</v>
+      </c>
+      <c r="F9" s="16">
+        <v>1</v>
+      </c>
+      <c r="G9" s="16">
+        <v>1</v>
+      </c>
+      <c r="H9" s="20">
+        <v>1</v>
+      </c>
+      <c r="I9" s="21"/>
+    </row>
+    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A10" s="16">
+        <v>1</v>
+      </c>
+      <c r="B10" s="16">
+        <v>1</v>
+      </c>
+      <c r="C10" s="20">
+        <v>1</v>
+      </c>
+      <c r="D10" s="16">
+        <v>0</v>
+      </c>
+      <c r="E10" s="17">
+        <v>1</v>
+      </c>
+      <c r="F10" s="16">
+        <v>0</v>
+      </c>
+      <c r="G10" s="16">
+        <v>0</v>
+      </c>
+      <c r="H10" s="20">
+        <v>1</v>
+      </c>
+      <c r="I10" s="21"/>
+    </row>
+    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A11" s="16">
+        <v>0</v>
+      </c>
+      <c r="B11" s="16">
+        <v>0</v>
+      </c>
+      <c r="C11" s="20">
+        <v>0</v>
+      </c>
+      <c r="D11" s="16">
+        <v>1</v>
+      </c>
+      <c r="E11" s="17">
+        <v>0</v>
+      </c>
+      <c r="F11" s="16">
+        <v>0</v>
+      </c>
+      <c r="G11" s="16">
+        <v>1</v>
+      </c>
+      <c r="H11" s="20">
+        <v>0</v>
+      </c>
+      <c r="I11" s="21"/>
+      <c r="J11" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="T11" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A12" s="16">
+        <v>0</v>
+      </c>
+      <c r="B12" s="16">
+        <v>0</v>
+      </c>
+      <c r="C12" s="20">
+        <v>1</v>
+      </c>
+      <c r="D12" s="16">
+        <v>1</v>
+      </c>
+      <c r="E12" s="17">
+        <v>0</v>
+      </c>
+      <c r="F12" s="16">
+        <v>0</v>
+      </c>
+      <c r="G12" s="16">
+        <v>1</v>
+      </c>
+      <c r="H12" s="20">
+        <v>0</v>
+      </c>
+      <c r="I12" s="21"/>
+      <c r="J12" s="13"/>
+      <c r="K12" s="11">
+        <v>0</v>
+      </c>
+      <c r="L12" s="11">
+        <v>1</v>
+      </c>
+      <c r="M12" s="11">
+        <v>11</v>
+      </c>
+      <c r="N12" s="11">
+        <v>10</v>
+      </c>
+      <c r="O12" s="11">
+        <v>110</v>
+      </c>
+      <c r="P12" s="11">
         <v>111</v>
       </c>
-      <c r="J2" s="5">
+      <c r="Q12" s="11">
+        <v>101</v>
+      </c>
+      <c r="R12" s="12">
+        <v>100</v>
+      </c>
+      <c r="T12" s="13"/>
+      <c r="U12" s="11">
+        <v>0</v>
+      </c>
+      <c r="V12" s="11">
+        <v>1</v>
+      </c>
+      <c r="W12" s="11">
+        <v>11</v>
+      </c>
+      <c r="X12" s="11">
+        <v>10</v>
+      </c>
+      <c r="Y12" s="11">
         <v>110</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="7"/>
-      <c r="B3" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="7"/>
-      <c r="B4" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="7"/>
-      <c r="B5" s="6">
+      <c r="Z12" s="11">
+        <v>111</v>
+      </c>
+      <c r="AA12" s="11">
+        <v>101</v>
+      </c>
+      <c r="AB12" s="12">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A13" s="16">
+        <v>0</v>
+      </c>
+      <c r="B13" s="16">
+        <v>1</v>
+      </c>
+      <c r="C13" s="20">
+        <v>0</v>
+      </c>
+      <c r="D13" s="16">
+        <v>1</v>
+      </c>
+      <c r="E13" s="17">
+        <v>0</v>
+      </c>
+      <c r="F13" s="16">
+        <v>1</v>
+      </c>
+      <c r="G13" s="16">
+        <v>0</v>
+      </c>
+      <c r="H13" s="20">
+        <v>0</v>
+      </c>
+      <c r="I13" s="21"/>
+      <c r="J13" s="14">
+        <v>0</v>
+      </c>
+      <c r="K13" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="L13" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="M13" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="N13" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="O13" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="P13" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q13" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="R13" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="T13" s="14">
+        <v>0</v>
+      </c>
+      <c r="U13" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="V13" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="W13" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="X13" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="Y13" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z13" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="AA13" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="AB13" s="19" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A14" s="16">
+        <v>0</v>
+      </c>
+      <c r="B14" s="16">
+        <v>1</v>
+      </c>
+      <c r="C14" s="20">
+        <v>1</v>
+      </c>
+      <c r="D14" s="16">
+        <v>1</v>
+      </c>
+      <c r="E14" s="17">
+        <v>0</v>
+      </c>
+      <c r="F14" s="16">
+        <v>1</v>
+      </c>
+      <c r="G14" s="16">
+        <v>0</v>
+      </c>
+      <c r="H14" s="20">
+        <v>0</v>
+      </c>
+      <c r="I14" s="21"/>
+      <c r="J14" s="14">
+        <v>1</v>
+      </c>
+      <c r="K14" s="5">
+        <v>0</v>
+      </c>
+      <c r="L14" s="5">
+        <v>1</v>
+      </c>
+      <c r="M14" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="N14" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="O14" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="P14" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q14" s="5">
+        <v>1</v>
+      </c>
+      <c r="R14" s="7">
+        <v>0</v>
+      </c>
+      <c r="T14" s="14">
+        <v>1</v>
+      </c>
+      <c r="U14" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="V14" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="W14" s="5">
+        <v>1</v>
+      </c>
+      <c r="X14" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y14" s="5">
+        <v>0</v>
+      </c>
+      <c r="Z14" s="5">
+        <v>1</v>
+      </c>
+      <c r="AA14" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AB14" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A15" s="16">
+        <v>1</v>
+      </c>
+      <c r="B15" s="16">
+        <v>0</v>
+      </c>
+      <c r="C15" s="20">
+        <v>0</v>
+      </c>
+      <c r="D15" s="16">
+        <v>1</v>
+      </c>
+      <c r="E15" s="17">
+        <v>0</v>
+      </c>
+      <c r="F15" s="16">
+        <v>1</v>
+      </c>
+      <c r="G15" s="16">
+        <v>1</v>
+      </c>
+      <c r="H15" s="20">
+        <v>0</v>
+      </c>
+      <c r="I15" s="21"/>
+      <c r="J15" s="14">
         <v>11</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="7"/>
-      <c r="B6" s="6">
+      <c r="K15" s="5">
+        <v>0</v>
+      </c>
+      <c r="L15" s="5">
+        <v>0</v>
+      </c>
+      <c r="M15" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="N15" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="O15" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="P15" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q15" s="5">
+        <v>0</v>
+      </c>
+      <c r="R15" s="7">
+        <v>0</v>
+      </c>
+      <c r="T15" s="14">
+        <v>11</v>
+      </c>
+      <c r="U15" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="V15" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="W15" s="5">
+        <v>0</v>
+      </c>
+      <c r="X15" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y15" s="5">
+        <v>0</v>
+      </c>
+      <c r="Z15" s="5">
+        <v>0</v>
+      </c>
+      <c r="AA15" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AB15" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A16" s="16">
+        <v>1</v>
+      </c>
+      <c r="B16" s="16">
+        <v>0</v>
+      </c>
+      <c r="C16" s="20">
+        <v>1</v>
+      </c>
+      <c r="D16" s="16">
+        <v>1</v>
+      </c>
+      <c r="E16" s="17">
+        <v>0</v>
+      </c>
+      <c r="F16" s="16">
+        <v>1</v>
+      </c>
+      <c r="G16" s="16">
+        <v>1</v>
+      </c>
+      <c r="H16" s="20">
+        <v>0</v>
+      </c>
+      <c r="I16" s="21"/>
+      <c r="J16" s="15">
         <v>10</v>
       </c>
+      <c r="K16" s="8">
+        <v>1</v>
+      </c>
+      <c r="L16" s="8">
+        <v>1</v>
+      </c>
+      <c r="M16" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="N16" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="O16" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="P16" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q16" s="8">
+        <v>1</v>
+      </c>
+      <c r="R16" s="9">
+        <v>1</v>
+      </c>
+      <c r="T16" s="15">
+        <v>10</v>
+      </c>
+      <c r="U16" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="V16" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="W16" s="8">
+        <v>1</v>
+      </c>
+      <c r="X16" s="8">
+        <v>1</v>
+      </c>
+      <c r="Y16" s="8">
+        <v>1</v>
+      </c>
+      <c r="Z16" s="8">
+        <v>1</v>
+      </c>
+      <c r="AA16" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="AB16" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A17" s="16">
+        <v>1</v>
+      </c>
+      <c r="B17" s="16">
+        <v>1</v>
+      </c>
+      <c r="C17" s="20">
+        <v>0</v>
+      </c>
+      <c r="D17" s="16">
+        <v>1</v>
+      </c>
+      <c r="E17" s="17">
+        <v>0</v>
+      </c>
+      <c r="F17" s="16">
+        <v>0</v>
+      </c>
+      <c r="G17" s="16">
+        <v>0</v>
+      </c>
+      <c r="H17" s="20">
+        <v>0</v>
+      </c>
+      <c r="I17" s="21"/>
+    </row>
+    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A18" s="16">
+        <v>1</v>
+      </c>
+      <c r="B18" s="16">
+        <v>1</v>
+      </c>
+      <c r="C18" s="20">
+        <v>1</v>
+      </c>
+      <c r="D18" s="16">
+        <v>1</v>
+      </c>
+      <c r="E18" s="17">
+        <v>0</v>
+      </c>
+      <c r="F18" s="16">
+        <v>0</v>
+      </c>
+      <c r="G18" s="16">
+        <v>0</v>
+      </c>
+      <c r="H18" s="20">
+        <v>0</v>
+      </c>
+      <c r="I18" s="21"/>
+    </row>
+    <row r="19" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A19" s="16">
+        <v>0</v>
+      </c>
+      <c r="B19" s="16">
+        <v>0</v>
+      </c>
+      <c r="C19" s="20">
+        <v>0</v>
+      </c>
+      <c r="D19" s="16">
+        <v>1</v>
+      </c>
+      <c r="E19" s="17">
+        <v>1</v>
+      </c>
+      <c r="F19" s="16">
+        <v>0</v>
+      </c>
+      <c r="G19" s="16">
+        <v>0</v>
+      </c>
+      <c r="H19" s="20">
+        <v>0</v>
+      </c>
+      <c r="I19" s="21"/>
+    </row>
+    <row r="20" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A20" s="16">
+        <v>0</v>
+      </c>
+      <c r="B20" s="16">
+        <v>0</v>
+      </c>
+      <c r="C20" s="20">
+        <v>1</v>
+      </c>
+      <c r="D20" s="16">
+        <v>1</v>
+      </c>
+      <c r="E20" s="17">
+        <v>1</v>
+      </c>
+      <c r="F20" s="16">
+        <v>0</v>
+      </c>
+      <c r="G20" s="16">
+        <v>0</v>
+      </c>
+      <c r="H20" s="20">
+        <v>1</v>
+      </c>
+      <c r="I20" s="21"/>
+      <c r="J20" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="T20" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A21" s="16">
+        <v>0</v>
+      </c>
+      <c r="B21" s="16">
+        <v>1</v>
+      </c>
+      <c r="C21" s="20">
+        <v>0</v>
+      </c>
+      <c r="D21" s="16">
+        <v>1</v>
+      </c>
+      <c r="E21" s="17">
+        <v>1</v>
+      </c>
+      <c r="F21" s="16">
+        <v>0</v>
+      </c>
+      <c r="G21" s="16">
+        <v>1</v>
+      </c>
+      <c r="H21" s="20">
+        <v>0</v>
+      </c>
+      <c r="I21" s="21"/>
+      <c r="J21" s="13"/>
+      <c r="K21" s="11">
+        <v>0</v>
+      </c>
+      <c r="L21" s="11">
+        <v>1</v>
+      </c>
+      <c r="M21" s="11">
+        <v>11</v>
+      </c>
+      <c r="N21" s="11">
+        <v>10</v>
+      </c>
+      <c r="O21" s="11">
+        <v>110</v>
+      </c>
+      <c r="P21" s="11">
+        <v>111</v>
+      </c>
+      <c r="Q21" s="11">
+        <v>101</v>
+      </c>
+      <c r="R21" s="12">
+        <v>100</v>
+      </c>
+      <c r="T21" s="13"/>
+      <c r="U21" s="11">
+        <v>0</v>
+      </c>
+      <c r="V21" s="11">
+        <v>1</v>
+      </c>
+      <c r="W21" s="11">
+        <v>11</v>
+      </c>
+      <c r="X21" s="11">
+        <v>10</v>
+      </c>
+      <c r="Y21" s="11">
+        <v>110</v>
+      </c>
+      <c r="Z21" s="11">
+        <v>111</v>
+      </c>
+      <c r="AA21" s="11">
+        <v>101</v>
+      </c>
+      <c r="AB21" s="12">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A22" s="16">
+        <v>0</v>
+      </c>
+      <c r="B22" s="16">
+        <v>1</v>
+      </c>
+      <c r="C22" s="20">
+        <v>1</v>
+      </c>
+      <c r="D22" s="16">
+        <v>1</v>
+      </c>
+      <c r="E22" s="17">
+        <v>1</v>
+      </c>
+      <c r="F22" s="16">
+        <v>0</v>
+      </c>
+      <c r="G22" s="16">
+        <v>1</v>
+      </c>
+      <c r="H22" s="20">
+        <v>1</v>
+      </c>
+      <c r="I22" s="21"/>
+      <c r="J22" s="14">
+        <v>0</v>
+      </c>
+      <c r="K22" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="L22" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="M22" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="N22" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="O22" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="P22" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q22" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="R22" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="T22" s="14">
+        <v>0</v>
+      </c>
+      <c r="U22" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="V22" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="W22" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="X22" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="Y22" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z22" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="AA22" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="AB22" s="19" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A23" s="16">
+        <v>1</v>
+      </c>
+      <c r="B23" s="16">
+        <v>0</v>
+      </c>
+      <c r="C23" s="20">
+        <v>0</v>
+      </c>
+      <c r="D23" s="16">
+        <v>1</v>
+      </c>
+      <c r="E23" s="17">
+        <v>1</v>
+      </c>
+      <c r="F23" s="16">
+        <v>1</v>
+      </c>
+      <c r="G23" s="16">
+        <v>0</v>
+      </c>
+      <c r="H23" s="20">
+        <v>0</v>
+      </c>
+      <c r="I23" s="21"/>
+      <c r="J23" s="14">
+        <v>1</v>
+      </c>
+      <c r="K23" s="5">
+        <v>1</v>
+      </c>
+      <c r="L23" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="M23" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="N23" s="5">
+        <v>1</v>
+      </c>
+      <c r="O23" s="5">
+        <v>1</v>
+      </c>
+      <c r="P23" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q23" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="R23" s="7">
+        <v>1</v>
+      </c>
+      <c r="T23" s="14">
+        <v>1</v>
+      </c>
+      <c r="U23" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="V23" s="5">
+        <v>0</v>
+      </c>
+      <c r="W23" s="5">
+        <v>0</v>
+      </c>
+      <c r="X23" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="Y23" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z23" s="5">
+        <v>0</v>
+      </c>
+      <c r="AA23" s="5">
+        <v>0</v>
+      </c>
+      <c r="AB23" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A24" s="16">
+        <v>1</v>
+      </c>
+      <c r="B24" s="16">
+        <v>0</v>
+      </c>
+      <c r="C24" s="20">
+        <v>1</v>
+      </c>
+      <c r="D24" s="16">
+        <v>1</v>
+      </c>
+      <c r="E24" s="17">
+        <v>1</v>
+      </c>
+      <c r="F24" s="16">
+        <v>1</v>
+      </c>
+      <c r="G24" s="16">
+        <v>0</v>
+      </c>
+      <c r="H24" s="20">
+        <v>1</v>
+      </c>
+      <c r="I24" s="21"/>
+      <c r="J24" s="14">
+        <v>11</v>
+      </c>
+      <c r="K24" s="5">
+        <v>0</v>
+      </c>
+      <c r="L24" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="M24" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="N24" s="5">
+        <v>0</v>
+      </c>
+      <c r="O24" s="5">
+        <v>0</v>
+      </c>
+      <c r="P24" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q24" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="R24" s="7">
+        <v>0</v>
+      </c>
+      <c r="T24" s="14">
+        <v>11</v>
+      </c>
+      <c r="U24" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="V24" s="5">
+        <v>0</v>
+      </c>
+      <c r="W24" s="5">
+        <v>0</v>
+      </c>
+      <c r="X24" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="Y24" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z24" s="5">
+        <v>0</v>
+      </c>
+      <c r="AA24" s="5">
+        <v>0</v>
+      </c>
+      <c r="AB24" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A25" s="16">
+        <v>1</v>
+      </c>
+      <c r="B25" s="16">
+        <v>1</v>
+      </c>
+      <c r="C25" s="20">
+        <v>0</v>
+      </c>
+      <c r="D25" s="16">
+        <v>1</v>
+      </c>
+      <c r="E25" s="17">
+        <v>1</v>
+      </c>
+      <c r="F25" s="16">
+        <v>1</v>
+      </c>
+      <c r="G25" s="16">
+        <v>1</v>
+      </c>
+      <c r="H25" s="20">
+        <v>0</v>
+      </c>
+      <c r="I25" s="21"/>
+      <c r="J25" s="15">
+        <v>10</v>
+      </c>
+      <c r="K25" s="8">
+        <v>0</v>
+      </c>
+      <c r="L25" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="M25" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="N25" s="8">
+        <v>0</v>
+      </c>
+      <c r="O25" s="8">
+        <v>0</v>
+      </c>
+      <c r="P25" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q25" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="R25" s="9">
+        <v>0</v>
+      </c>
+      <c r="T25" s="15">
+        <v>10</v>
+      </c>
+      <c r="U25" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="V25" s="8">
+        <v>1</v>
+      </c>
+      <c r="W25" s="8">
+        <v>1</v>
+      </c>
+      <c r="X25" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="Y25" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z25" s="8">
+        <v>1</v>
+      </c>
+      <c r="AA25" s="8">
+        <v>1</v>
+      </c>
+      <c r="AB25" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A26" s="16">
+        <v>1</v>
+      </c>
+      <c r="B26" s="16">
+        <v>1</v>
+      </c>
+      <c r="C26" s="20">
+        <v>1</v>
+      </c>
+      <c r="D26" s="16">
+        <v>1</v>
+      </c>
+      <c r="E26" s="17">
+        <v>1</v>
+      </c>
+      <c r="F26" s="16">
+        <v>1</v>
+      </c>
+      <c r="G26" s="16">
+        <v>1</v>
+      </c>
+      <c r="H26" s="20">
+        <v>1</v>
+      </c>
+      <c r="I26" s="21"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>